<commit_message>
Add results tables in excel - these are converted to latex for the paper
</commit_message>
<xml_diff>
--- a/paper/results/SimulatedDataSets.xlsx
+++ b/paper/results/SimulatedDataSets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="52000" yWindow="11720" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="52380" yWindow="9060" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,24 +19,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Error Rate</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Total Reads</t>
   </si>
   <si>
-    <t>Reads with Adapters</t>
-  </si>
-  <si>
     <t>Data Set</t>
   </si>
   <si>
     <t>Read Length</t>
   </si>
   <si>
-    <t>Adapter Bases</t>
+    <t>Simulated 1</t>
+  </si>
+  <si>
+    <t>Simulated 2</t>
+  </si>
+  <si>
+    <t>Simulated 3</t>
+  </si>
+  <si>
+    <t>GM12878 WGBS</t>
+  </si>
+  <si>
+    <t>Error Rate*</t>
+  </si>
+  <si>
+    <t>Reads with Adapters*</t>
+  </si>
+  <si>
+    <t>Adapter Bases*</t>
   </si>
 </sst>
 </file>
@@ -76,7 +88,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -84,8 +96,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -93,20 +114,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -436,82 +471,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="20.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+      <c r="D1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>1</v>
+      <c r="A2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>125</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
+        <v>781923</v>
+      </c>
+      <c r="D2" s="2">
         <v>2E-3</v>
       </c>
-      <c r="D2" s="3">
-        <v>781923</v>
-      </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="4">
+        <v>325982</v>
+      </c>
+      <c r="F2" s="5">
+        <v>12447262</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1">
-        <v>2</v>
+      <c r="A3" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>125</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
+        <v>780899</v>
+      </c>
+      <c r="D3" s="2">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D3" s="3">
-        <v>780899</v>
-      </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="4">
+        <v>325105</v>
+      </c>
+      <c r="F3" s="5">
+        <v>12416861</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1">
-        <v>3</v>
+      <c r="A4" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B4" s="1">
         <v>125</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
+        <v>782237</v>
+      </c>
+      <c r="D4" s="2">
         <v>1.2E-2</v>
       </c>
-      <c r="D4" s="3">
-        <v>782237</v>
-      </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="4">
+        <v>325860</v>
+      </c>
+      <c r="F4" s="5">
+        <v>12464235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>125</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1000000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add latex version of table of data sets
</commit_message>
<xml_diff>
--- a/paper/results/SimulatedDataSets.xlsx
+++ b/paper/results/SimulatedDataSets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="52380" yWindow="9060" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="54560" yWindow="1740" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Error Rate</t>
+  </si>
   <si>
     <t>Total Reads</t>
   </si>
@@ -30,6 +33,9 @@
     <t>Read Length</t>
   </si>
   <si>
+    <t>Adapter Bases</t>
+  </si>
+  <si>
     <t>Simulated 1</t>
   </si>
   <si>
@@ -42,13 +48,16 @@
     <t>GM12878 WGBS</t>
   </si>
   <si>
-    <t>Error Rate*</t>
-  </si>
-  <si>
-    <t>Reads with Adapters*</t>
-  </si>
-  <si>
-    <t>Adapter Bases*</t>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>16,999*</t>
+  </si>
+  <si>
+    <t>1,020,017*</t>
+  </si>
+  <si>
+    <t>Reads w/ Adapters</t>
   </si>
 </sst>
 </file>
@@ -106,7 +115,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -118,30 +127,46 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -474,105 +499,116 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="5"/>
+    <col min="3" max="3" width="11.5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
+        <v>5</v>
+      </c>
+      <c r="B2" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="C2" s="5">
         <v>125</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="2">
         <v>781923</v>
       </c>
-      <c r="D2" s="2">
-        <v>2E-3</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>325982</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>12447262</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
+        <v>6</v>
+      </c>
+      <c r="B3" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C3" s="5">
         <v>125</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="2">
         <v>780899</v>
       </c>
-      <c r="D3" s="2">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>325105</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>12416861</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
+        <v>7</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C4" s="5">
         <v>125</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="2">
         <v>782237</v>
       </c>
-      <c r="D4" s="2">
-        <v>1.2E-2</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>325860</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>12464235</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5">
         <v>125</v>
       </c>
-      <c r="C5" s="5">
+      <c r="D5" s="4">
         <v>1000000</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>